<commit_message>
Did the force sensor testing
</commit_message>
<xml_diff>
--- a/Electrical/Force Sensor Validation.xlsx
+++ b/Electrical/Force Sensor Validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiara\Desktop\Projects\Gripper Arm - ROBOTICS CLUB\Gripper-Arm\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2805DAFC-B16A-493E-BFF1-701C18FD97FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1A8421-4A40-49A1-B3C3-1DD1E5D3D605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{50B44107-D503-4282-AD0F-5DEE1A6A2725}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Equipment Used</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Multimeter - FLUKE 117</t>
   </si>
   <si>
-    <t>Applied Force [N]</t>
-  </si>
-  <si>
     <t>Resistance [Ohms]</t>
   </si>
   <si>
@@ -46,6 +43,12 @@
   </si>
   <si>
     <t>Sensor 2</t>
+  </si>
+  <si>
+    <t>Applied Force [kg]</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -397,97 +400,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13F572A-E3F5-41F4-AA53-618F57706A74}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="23.76953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <v>150000</v>
+      </c>
+      <c r="E3">
+        <v>0.2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="C4">
+        <v>0.4</v>
+      </c>
+      <c r="D4">
+        <v>30000</v>
+      </c>
+      <c r="E4">
+        <v>0.4</v>
+      </c>
+      <c r="F4">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+      <c r="D5">
+        <v>8000</v>
+      </c>
+      <c r="E5">
+        <v>0.6</v>
+      </c>
+      <c r="F5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="C6">
+        <v>0.8</v>
+      </c>
+      <c r="D6">
+        <v>7900</v>
+      </c>
+      <c r="E6">
+        <v>0.8</v>
+      </c>
+      <c r="F6">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C4">
+      <c r="D7">
+        <v>6000</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2000</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <f>0.5*1000</f>
+        <v>500</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>450</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="C11">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C9">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C11">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C12">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="C13">
-        <v>50</v>
+      <c r="D11">
+        <v>230</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished sensor feedback for FSRs
</commit_message>
<xml_diff>
--- a/Electrical/Force Sensor Validation.xlsx
+++ b/Electrical/Force Sensor Validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiara\Desktop\Projects\Gripper Arm - ROBOTICS CLUB\Gripper-Arm\Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gripper-Arm\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1A8421-4A40-49A1-B3C3-1DD1E5D3D605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E59539-FF25-4DF2-8681-F46A2B4AC1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{50B44107-D503-4282-AD0F-5DEE1A6A2725}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50B44107-D503-4282-AD0F-5DEE1A6A2725}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Equipment Used</t>
   </si>
@@ -49,6 +60,24 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Voltage Divider Calculations</t>
+  </si>
+  <si>
+    <t>Resistance (Force Sensor)</t>
+  </si>
+  <si>
+    <t>R2 Resistance</t>
+  </si>
+  <si>
+    <t>Input Voltage</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Resolution</t>
   </si>
 </sst>
 </file>
@@ -400,22 +429,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13F572A-E3F5-41F4-AA53-618F57706A74}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.76953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,8 +458,17 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -442,8 +484,20 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -459,8 +513,18 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="J3">
+        <v>150000</v>
+      </c>
+      <c r="K3">
+        <v>3300</v>
+      </c>
+      <c r="L3">
+        <f>($M$1*K3)/(J3+K3)</f>
+        <v>0.10763209393346379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>0.4</v>
       </c>
@@ -473,8 +537,22 @@
       <c r="F4">
         <v>24000</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="J4">
+        <v>145000</v>
+      </c>
+      <c r="K4">
+        <v>3300</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L41" si="0">($M$1*K4)/(J4+K4)</f>
+        <v>0.11126095751854349</v>
+      </c>
+      <c r="M4">
+        <f>L4-L3</f>
+        <v>3.628863585079703E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>0.6</v>
       </c>
@@ -487,8 +565,22 @@
       <c r="F5">
         <v>10000</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="J5">
+        <v>140000</v>
+      </c>
+      <c r="K5">
+        <v>3300</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0.1151430565247732</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M41" si="1">L5-L4</f>
+        <v>3.8820990062297112E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>0.8</v>
       </c>
@@ -501,8 +593,22 @@
       <c r="F6">
         <v>6000</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="J6">
+        <v>135000</v>
+      </c>
+      <c r="K6">
+        <v>3300</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.1193058568329718</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>4.1628003081985998E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1</v>
       </c>
@@ -515,8 +621,22 @@
       <c r="F7">
         <v>5900</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="J7">
+        <v>130000</v>
+      </c>
+      <c r="K7">
+        <v>3300</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.12378094523630907</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>4.4750884033372684E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>2</v>
       </c>
@@ -529,8 +649,22 @@
       <c r="F8">
         <v>1500</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="J8">
+        <v>125000</v>
+      </c>
+      <c r="K8">
+        <v>3300</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0.12860483242400625</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>4.8238871876971762E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>3</v>
       </c>
@@ -544,8 +678,22 @@
       <c r="F9">
         <v>1000</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="J9">
+        <v>120000</v>
+      </c>
+      <c r="K9">
+        <v>3300</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0.13381995133819952</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>5.2151189141932675E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>4</v>
       </c>
@@ -558,8 +706,22 @@
       <c r="F10">
         <v>600</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="J10">
+        <v>115000</v>
+      </c>
+      <c r="K10">
+        <v>3300</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0.13947590870667795</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>5.6559573684784314E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>5</v>
       </c>
@@ -571,6 +733,500 @@
       </c>
       <c r="F11" t="s">
         <v>7</v>
+      </c>
+      <c r="J11">
+        <v>110000</v>
+      </c>
+      <c r="K11">
+        <v>3300</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0.14563106796116504</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>6.1551592544870914E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>105000</v>
+      </c>
+      <c r="K12">
+        <v>3300</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0.1523545706371191</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>6.7235026759540628E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>100000</v>
+      </c>
+      <c r="K13">
+        <v>3300</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>0.15972894482090996</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>7.3743741837908605E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>95000</v>
+      </c>
+      <c r="K14">
+        <v>3300</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0.16785350966429299</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>8.1245648433830309E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>90000</v>
+      </c>
+      <c r="K15">
+        <v>3300</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0.17684887459807075</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>8.9953649337777553E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>85000</v>
+      </c>
+      <c r="K16">
+        <v>3300</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0.1868629671574179</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>1.0014092559347154E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>80000</v>
+      </c>
+      <c r="K17">
+        <v>3300</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>0.19807923169267708</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>1.1216264535259174E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>75000</v>
+      </c>
+      <c r="K18">
+        <v>3300</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>0.21072796934865901</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>1.2648737655981929E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>70000</v>
+      </c>
+      <c r="K19">
+        <v>3300</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>0.22510231923601637</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>1.4374349887357363E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>65000</v>
+      </c>
+      <c r="K20">
+        <v>3300</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>0.24158125915080528</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>1.6478939914788909E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>60000</v>
+      </c>
+      <c r="K21">
+        <v>3300</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>0.26066350710900477</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>1.9082247958199489E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>55000</v>
+      </c>
+      <c r="K22">
+        <v>3300</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>0.28301886792452829</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>2.2355360815523528E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>50000</v>
+      </c>
+      <c r="K23">
+        <v>3300</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>0.30956848030018763</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>2.6549612375659337E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>45000</v>
+      </c>
+      <c r="K24">
+        <v>3300</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>0.34161490683229812</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>3.2046426532110484E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>40000</v>
+      </c>
+      <c r="K25">
+        <v>3300</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>0.38106235565819863</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>3.9447448825900511E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>35000</v>
+      </c>
+      <c r="K26">
+        <v>3300</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>0.43080939947780678</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>4.974704381960815E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>30000</v>
+      </c>
+      <c r="K27">
+        <v>3300</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>0.49549549549549549</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>6.468609601768871E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>25000</v>
+      </c>
+      <c r="K28">
+        <v>3300</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>0.58303886925795056</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>8.7543373762455079E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>20000</v>
+      </c>
+      <c r="K29">
+        <v>3300</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>0.70815450643776823</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>0.12511563717981766</v>
+      </c>
+    </row>
+    <row r="30" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>15000</v>
+      </c>
+      <c r="K30">
+        <v>3300</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>0.90163934426229508</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>0.19348483782452686</v>
+      </c>
+    </row>
+    <row r="31" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>10000</v>
+      </c>
+      <c r="K31">
+        <v>3300</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>1.2406015037593985</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>0.3389621594971034</v>
+      </c>
+    </row>
+    <row r="32" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>5000</v>
+      </c>
+      <c r="K32">
+        <v>3300</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>1.9879518072289157</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>0.74735030346951725</v>
+      </c>
+    </row>
+    <row r="33" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>4000</v>
+      </c>
+      <c r="K33">
+        <v>3300</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>2.2602739726027399</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>0.27232216537382414</v>
+      </c>
+    </row>
+    <row r="34" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>3000</v>
+      </c>
+      <c r="K34">
+        <v>3300</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>2.6190476190476191</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>0.35877364644487919</v>
+      </c>
+    </row>
+    <row r="35" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <v>2000</v>
+      </c>
+      <c r="K35">
+        <v>3300</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>3.1132075471698113</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="1"/>
+        <v>0.49415992812219223</v>
+      </c>
+    </row>
+    <row r="36" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <v>1000</v>
+      </c>
+      <c r="K36">
+        <v>3300</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>3.8372093023255816</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="1"/>
+        <v>0.72400175515577025</v>
+      </c>
+    </row>
+    <row r="37" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>750</v>
+      </c>
+      <c r="K37">
+        <v>3300</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="0"/>
+        <v>4.0740740740740744</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="1"/>
+        <v>0.23686477174849285</v>
+      </c>
+    </row>
+    <row r="38" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <v>500</v>
+      </c>
+      <c r="K38">
+        <v>3300</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="0"/>
+        <v>4.3421052631578947</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="1"/>
+        <v>0.26803118908382029</v>
+      </c>
+    </row>
+    <row r="39" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <v>250</v>
+      </c>
+      <c r="K39">
+        <v>3300</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="0"/>
+        <v>4.647887323943662</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="1"/>
+        <v>0.30578206078576731</v>
+      </c>
+    </row>
+    <row r="40" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <v>100</v>
+      </c>
+      <c r="K40">
+        <v>3300</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="0"/>
+        <v>4.8529411764705879</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="1"/>
+        <v>0.20505385252692587</v>
+      </c>
+    </row>
+    <row r="41" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <v>50</v>
+      </c>
+      <c r="K41">
+        <v>3300</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>4.9253731343283578</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="1"/>
+        <v>7.2431957857769902E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed all schematics initially
gonna wait on review
</commit_message>
<xml_diff>
--- a/Electrical/Force Sensor Validation.xlsx
+++ b/Electrical/Force Sensor Validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gripper-Arm\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E59539-FF25-4DF2-8681-F46A2B4AC1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E53850-ADD3-46AA-9297-36762D664CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50B44107-D503-4282-AD0F-5DEE1A6A2725}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +465,7 @@
         <v>11</v>
       </c>
       <c r="M1">
-        <v>5</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -517,11 +517,11 @@
         <v>150000</v>
       </c>
       <c r="K3">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L3">
         <f>($M$1*K3)/(J3+K3)</f>
-        <v>0.10763209393346379</v>
+        <v>0.20624999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -541,15 +541,15 @@
         <v>145000</v>
       </c>
       <c r="K4">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L41" si="0">($M$1*K4)/(J4+K4)</f>
-        <v>0.11126095751854349</v>
+        <v>0.2129032258064516</v>
       </c>
       <c r="M4">
         <f>L4-L3</f>
-        <v>3.628863585079703E-3</v>
+        <v>6.6532258064516125E-3</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -569,15 +569,15 @@
         <v>140000</v>
       </c>
       <c r="K5">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>0.1151430565247732</v>
+        <v>0.22</v>
       </c>
       <c r="M5">
         <f t="shared" ref="M5:M41" si="1">L5-L4</f>
-        <v>3.8820990062297112E-3</v>
+        <v>7.0967741935483997E-3</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -597,15 +597,15 @@
         <v>135000</v>
       </c>
       <c r="K6">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>0.1193058568329718</v>
+        <v>0.22758620689655173</v>
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>4.1628003081985998E-3</v>
+        <v>7.5862068965517337E-3</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -625,15 +625,15 @@
         <v>130000</v>
       </c>
       <c r="K7">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>0.12378094523630907</v>
+        <v>0.23571428571428571</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>4.4750884033372684E-3</v>
+        <v>8.1280788177339747E-3</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -653,15 +653,15 @@
         <v>125000</v>
       </c>
       <c r="K8">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>0.12860483242400625</v>
+        <v>0.24444444444444444</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>4.8238871876971762E-3</v>
+        <v>8.7301587301587269E-3</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -682,15 +682,15 @@
         <v>120000</v>
       </c>
       <c r="K9">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>0.13381995133819952</v>
+        <v>0.25384615384615383</v>
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
-        <v>5.2151189141932675E-3</v>
+        <v>9.4017094017093961E-3</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -710,15 +710,15 @@
         <v>115000</v>
       </c>
       <c r="K10">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>0.13947590870667795</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
-        <v>5.6559573684784314E-3</v>
+        <v>1.015384615384618E-2</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -738,15 +738,15 @@
         <v>110000</v>
       </c>
       <c r="K11">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>0.14563106796116504</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>6.1551592544870914E-3</v>
+        <v>1.100000000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -754,15 +754,15 @@
         <v>105000</v>
       </c>
       <c r="K12">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>0.1523545706371191</v>
+        <v>0.28695652173913044</v>
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>6.7235026759540628E-3</v>
+        <v>1.1956521739130421E-2</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -770,15 +770,15 @@
         <v>100000</v>
       </c>
       <c r="K13">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>0.15972894482090996</v>
+        <v>0.3</v>
       </c>
       <c r="M13">
         <f t="shared" si="1"/>
-        <v>7.3743741837908605E-3</v>
+        <v>1.3043478260869545E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -786,15 +786,15 @@
         <v>95000</v>
       </c>
       <c r="K14">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>0.16785350966429299</v>
+        <v>0.31428571428571428</v>
       </c>
       <c r="M14">
         <f t="shared" si="1"/>
-        <v>8.1245648433830309E-3</v>
+        <v>1.428571428571429E-2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -802,15 +802,15 @@
         <v>90000</v>
       </c>
       <c r="K15">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>0.17684887459807075</v>
+        <v>0.33</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>8.9953649337777553E-3</v>
+        <v>1.5714285714285736E-2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -818,15 +818,15 @@
         <v>85000</v>
       </c>
       <c r="K16">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L16">
         <f t="shared" si="0"/>
-        <v>0.1868629671574179</v>
+        <v>0.3473684210526316</v>
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
-        <v>1.0014092559347154E-2</v>
+        <v>1.7368421052631589E-2</v>
       </c>
     </row>
     <row r="17" spans="10:13" x14ac:dyDescent="0.25">
@@ -834,15 +834,15 @@
         <v>80000</v>
       </c>
       <c r="K17">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
-        <v>0.19807923169267708</v>
+        <v>0.36666666666666664</v>
       </c>
       <c r="M17">
         <f t="shared" si="1"/>
-        <v>1.1216264535259174E-2</v>
+        <v>1.9298245614035037E-2</v>
       </c>
     </row>
     <row r="18" spans="10:13" x14ac:dyDescent="0.25">
@@ -850,15 +850,15 @@
         <v>75000</v>
       </c>
       <c r="K18">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>0.21072796934865901</v>
+        <v>0.38823529411764707</v>
       </c>
       <c r="M18">
         <f t="shared" si="1"/>
-        <v>1.2648737655981929E-2</v>
+        <v>2.1568627450980427E-2</v>
       </c>
     </row>
     <row r="19" spans="10:13" x14ac:dyDescent="0.25">
@@ -866,15 +866,15 @@
         <v>70000</v>
       </c>
       <c r="K19">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>0.22510231923601637</v>
+        <v>0.41249999999999998</v>
       </c>
       <c r="M19">
         <f t="shared" si="1"/>
-        <v>1.4374349887357363E-2</v>
+        <v>2.426470588235291E-2</v>
       </c>
     </row>
     <row r="20" spans="10:13" x14ac:dyDescent="0.25">
@@ -882,15 +882,15 @@
         <v>65000</v>
       </c>
       <c r="K20">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L20">
         <f t="shared" si="0"/>
-        <v>0.24158125915080528</v>
+        <v>0.44</v>
       </c>
       <c r="M20">
         <f t="shared" si="1"/>
-        <v>1.6478939914788909E-2</v>
+        <v>2.7500000000000024E-2</v>
       </c>
     </row>
     <row r="21" spans="10:13" x14ac:dyDescent="0.25">
@@ -898,15 +898,15 @@
         <v>60000</v>
       </c>
       <c r="K21">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L21">
         <f t="shared" si="0"/>
-        <v>0.26066350710900477</v>
+        <v>0.47142857142857142</v>
       </c>
       <c r="M21">
         <f t="shared" si="1"/>
-        <v>1.9082247958199489E-2</v>
+        <v>3.1428571428571417E-2</v>
       </c>
     </row>
     <row r="22" spans="10:13" x14ac:dyDescent="0.25">
@@ -914,15 +914,15 @@
         <v>55000</v>
       </c>
       <c r="K22">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L22">
         <f t="shared" si="0"/>
-        <v>0.28301886792452829</v>
+        <v>0.50769230769230766</v>
       </c>
       <c r="M22">
         <f t="shared" si="1"/>
-        <v>2.2355360815523528E-2</v>
+        <v>3.6263736263736246E-2</v>
       </c>
     </row>
     <row r="23" spans="10:13" x14ac:dyDescent="0.25">
@@ -930,15 +930,15 @@
         <v>50000</v>
       </c>
       <c r="K23">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>0.30956848030018763</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M23">
         <f t="shared" si="1"/>
-        <v>2.6549612375659337E-2</v>
+        <v>4.2307692307692379E-2</v>
       </c>
     </row>
     <row r="24" spans="10:13" x14ac:dyDescent="0.25">
@@ -946,15 +946,15 @@
         <v>45000</v>
       </c>
       <c r="K24">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L24">
         <f t="shared" si="0"/>
-        <v>0.34161490683229812</v>
+        <v>0.6</v>
       </c>
       <c r="M24">
         <f t="shared" si="1"/>
-        <v>3.2046426532110484E-2</v>
+        <v>4.9999999999999933E-2</v>
       </c>
     </row>
     <row r="25" spans="10:13" x14ac:dyDescent="0.25">
@@ -962,15 +962,15 @@
         <v>40000</v>
       </c>
       <c r="K25">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
-        <v>0.38106235565819863</v>
+        <v>0.66</v>
       </c>
       <c r="M25">
         <f t="shared" si="1"/>
-        <v>3.9447448825900511E-2</v>
+        <v>6.0000000000000053E-2</v>
       </c>
     </row>
     <row r="26" spans="10:13" x14ac:dyDescent="0.25">
@@ -978,15 +978,15 @@
         <v>35000</v>
       </c>
       <c r="K26">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L26">
         <f t="shared" si="0"/>
-        <v>0.43080939947780678</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="M26">
         <f t="shared" si="1"/>
-        <v>4.974704381960815E-2</v>
+        <v>7.333333333333325E-2</v>
       </c>
     </row>
     <row r="27" spans="10:13" x14ac:dyDescent="0.25">
@@ -994,15 +994,15 @@
         <v>30000</v>
       </c>
       <c r="K27">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L27">
         <f t="shared" si="0"/>
-        <v>0.49549549549549549</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="M27">
         <f t="shared" si="1"/>
-        <v>6.468609601768871E-2</v>
+        <v>9.1666666666666674E-2</v>
       </c>
     </row>
     <row r="28" spans="10:13" x14ac:dyDescent="0.25">
@@ -1010,15 +1010,15 @@
         <v>25000</v>
       </c>
       <c r="K28">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L28">
         <f t="shared" si="0"/>
-        <v>0.58303886925795056</v>
+        <v>0.94285714285714284</v>
       </c>
       <c r="M28">
         <f t="shared" si="1"/>
-        <v>8.7543373762455079E-2</v>
+        <v>0.11785714285714288</v>
       </c>
     </row>
     <row r="29" spans="10:13" x14ac:dyDescent="0.25">
@@ -1026,15 +1026,15 @@
         <v>20000</v>
       </c>
       <c r="K29">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L29">
         <f t="shared" si="0"/>
-        <v>0.70815450643776823</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M29">
         <f t="shared" si="1"/>
-        <v>0.12511563717981766</v>
+        <v>0.15714285714285725</v>
       </c>
     </row>
     <row r="30" spans="10:13" x14ac:dyDescent="0.25">
@@ -1042,15 +1042,15 @@
         <v>15000</v>
       </c>
       <c r="K30">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
-        <v>0.90163934426229508</v>
+        <v>1.32</v>
       </c>
       <c r="M30">
         <f t="shared" si="1"/>
-        <v>0.19348483782452686</v>
+        <v>0.21999999999999997</v>
       </c>
     </row>
     <row r="31" spans="10:13" x14ac:dyDescent="0.25">
@@ -1058,15 +1058,15 @@
         <v>10000</v>
       </c>
       <c r="K31">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L31">
         <f t="shared" si="0"/>
-        <v>1.2406015037593985</v>
+        <v>1.65</v>
       </c>
       <c r="M31">
         <f t="shared" si="1"/>
-        <v>0.3389621594971034</v>
+        <v>0.32999999999999985</v>
       </c>
     </row>
     <row r="32" spans="10:13" x14ac:dyDescent="0.25">
@@ -1074,15 +1074,15 @@
         <v>5000</v>
       </c>
       <c r="K32">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>1.9879518072289157</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M32">
         <f t="shared" si="1"/>
-        <v>0.74735030346951725</v>
+        <v>0.55000000000000027</v>
       </c>
     </row>
     <row r="33" spans="10:13" x14ac:dyDescent="0.25">
@@ -1090,15 +1090,15 @@
         <v>4000</v>
       </c>
       <c r="K33">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L33">
         <f t="shared" si="0"/>
-        <v>2.2602739726027399</v>
+        <v>2.3571428571428572</v>
       </c>
       <c r="M33">
         <f t="shared" si="1"/>
-        <v>0.27232216537382414</v>
+        <v>0.15714285714285703</v>
       </c>
     </row>
     <row r="34" spans="10:13" x14ac:dyDescent="0.25">
@@ -1106,15 +1106,15 @@
         <v>3000</v>
       </c>
       <c r="K34">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L34">
         <f t="shared" si="0"/>
-        <v>2.6190476190476191</v>
+        <v>2.5384615384615383</v>
       </c>
       <c r="M34">
         <f t="shared" si="1"/>
-        <v>0.35877364644487919</v>
+        <v>0.18131868131868112</v>
       </c>
     </row>
     <row r="35" spans="10:13" x14ac:dyDescent="0.25">
@@ -1122,15 +1122,15 @@
         <v>2000</v>
       </c>
       <c r="K35">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
-        <v>3.1132075471698113</v>
+        <v>2.75</v>
       </c>
       <c r="M35">
         <f t="shared" si="1"/>
-        <v>0.49415992812219223</v>
+        <v>0.21153846153846168</v>
       </c>
     </row>
     <row r="36" spans="10:13" x14ac:dyDescent="0.25">
@@ -1138,15 +1138,15 @@
         <v>1000</v>
       </c>
       <c r="K36">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L36">
         <f t="shared" si="0"/>
-        <v>3.8372093023255816</v>
+        <v>3</v>
       </c>
       <c r="M36">
         <f t="shared" si="1"/>
-        <v>0.72400175515577025</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="37" spans="10:13" x14ac:dyDescent="0.25">
@@ -1154,15 +1154,15 @@
         <v>750</v>
       </c>
       <c r="K37">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L37">
         <f t="shared" si="0"/>
-        <v>4.0740740740740744</v>
+        <v>3.0697674418604652</v>
       </c>
       <c r="M37">
         <f t="shared" si="1"/>
-        <v>0.23686477174849285</v>
+        <v>6.976744186046524E-2</v>
       </c>
     </row>
     <row r="38" spans="10:13" x14ac:dyDescent="0.25">
@@ -1170,15 +1170,15 @@
         <v>500</v>
       </c>
       <c r="K38">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L38">
         <f t="shared" si="0"/>
-        <v>4.3421052631578947</v>
+        <v>3.1428571428571428</v>
       </c>
       <c r="M38">
         <f t="shared" si="1"/>
-        <v>0.26803118908382029</v>
+        <v>7.3089700996677553E-2</v>
       </c>
     </row>
     <row r="39" spans="10:13" x14ac:dyDescent="0.25">
@@ -1186,15 +1186,15 @@
         <v>250</v>
       </c>
       <c r="K39">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L39">
         <f t="shared" si="0"/>
-        <v>4.647887323943662</v>
+        <v>3.2195121951219514</v>
       </c>
       <c r="M39">
         <f t="shared" si="1"/>
-        <v>0.30578206078576731</v>
+        <v>7.6655052264808621E-2</v>
       </c>
     </row>
     <row r="40" spans="10:13" x14ac:dyDescent="0.25">
@@ -1202,15 +1202,15 @@
         <v>100</v>
       </c>
       <c r="K40">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L40">
         <f t="shared" si="0"/>
-        <v>4.8529411764705879</v>
+        <v>3.2673267326732671</v>
       </c>
       <c r="M40">
         <f t="shared" si="1"/>
-        <v>0.20505385252692587</v>
+        <v>4.7814537551315706E-2</v>
       </c>
     </row>
     <row r="41" spans="10:13" x14ac:dyDescent="0.25">
@@ -1218,15 +1218,15 @@
         <v>50</v>
       </c>
       <c r="K41">
-        <v>3300</v>
+        <v>10000</v>
       </c>
       <c r="L41">
         <f t="shared" si="0"/>
-        <v>4.9253731343283578</v>
+        <v>3.283582089552239</v>
       </c>
       <c r="M41">
         <f t="shared" si="1"/>
-        <v>7.2431957857769902E-2</v>
+        <v>1.6255356878971838E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>